<commit_message>
fix: delete contam_prop from data in usedata vignette 3.2
</commit_message>
<xml_diff>
--- a/vignettes/results/BMF_computation_PCB_ng_glw/2.BMF_diet_all_PCB_ng_glw.xlsx
+++ b/vignettes/results/BMF_computation_PCB_ng_glw/2.BMF_diet_all_PCB_ng_glw.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,41 +408,6 @@
           <t>BMF_diet_max</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>chem_label</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>family</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>sub_family_TAG</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>sub_family_name</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>logKow</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>n_C</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>LOQ_biote</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -477,24 +442,6 @@
       <c r="J2">
         <v>2.942007481805241</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>CB-101</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="O2">
-        <v>6.38</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -529,24 +476,6 @@
       <c r="J3">
         <v>3.017217569820718</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>CB-105</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="O3">
-        <v>6.65</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -581,24 +510,6 @@
       <c r="J4">
         <v>3.067853096449863</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>CB-110</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="O4">
-        <v>6.48</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -633,24 +544,6 @@
       <c r="J5">
         <v>2.891729796920242</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>CB-118</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="O5">
-        <v>6.74</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -685,24 +578,6 @@
       <c r="J6">
         <v>2.948740069123974</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>CB-128</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O6">
-        <v>6.74</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -737,24 +612,6 @@
       <c r="J7">
         <v>2.164040146353941</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>CB-132</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O7">
-        <v>6.58</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -789,24 +646,6 @@
       <c r="J8">
         <v>2.977886417764166</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>CB-138</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O8">
-        <v>6.83</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -841,24 +680,6 @@
       <c r="J9">
         <v>2.194328237194325</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>CB-149</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O9">
-        <v>6.67</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -893,24 +714,6 @@
       <c r="J10">
         <v>2.676121257753783</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>CB-153</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O10">
-        <v>6.92</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -945,24 +748,6 @@
       <c r="J11">
         <v>1.346262734169168</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>CB-156</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="O11">
-        <v>7.18</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -997,24 +782,6 @@
       <c r="J12">
         <v>2.22273613504151</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>CB-170</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>hepta-CB</t>
-        </is>
-      </c>
-      <c r="O12">
-        <v>7.11</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1049,24 +816,6 @@
       <c r="J13">
         <v>2.768445273999823</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>CB-180</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>hepta-CB</t>
-        </is>
-      </c>
-      <c r="O13">
-        <v>7.36</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1101,24 +850,6 @@
       <c r="J14">
         <v>1.525153103101246</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>CB-028</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>tri-CB</t>
-        </is>
-      </c>
-      <c r="O14">
-        <v>5.67</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1153,24 +884,6 @@
       <c r="J15">
         <v>0.9314676918829942</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>CB-031</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>tri-CB</t>
-        </is>
-      </c>
-      <c r="O15">
-        <v>5.67</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1205,24 +918,6 @@
       <c r="J16">
         <v>2.442778417042918</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>CB-044</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="O16">
-        <v>5.75</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1257,24 +952,6 @@
       <c r="J17">
         <v>2.517602804494201</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>CB-049</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="O17">
-        <v>5.63</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1308,24 +985,6 @@
       </c>
       <c r="J18">
         <v>2.657111708822246</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>CB-052</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="O18">
-        <v>5.84</v>
       </c>
     </row>
     <row r="19">

</xml_diff>